<commit_message>
[feat] users list updated
</commit_message>
<xml_diff>
--- a/instagram_threads_bulk_block_unblock/list/users.xlsx
+++ b/instagram_threads_bulk_block_unblock/list/users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muffafa/Desktop/deneme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muffafa/Desktop/awesome_basic_tools_for_social_media/instagram_threads_bulk_block_unblock/list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8716D4BF-F60D-1C45-B023-F0D68675CEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012D9D5A-7F77-9F4F-9588-77CA370F5DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{B89FE81D-986D-1A44-B73A-18C67171BAD0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>usernames</t>
   </si>
@@ -45,6 +45,234 @@
   </si>
   <si>
     <t>muratcanicdag</t>
+  </si>
+  <si>
+    <t>cagritaner</t>
+  </si>
+  <si>
+    <t>huzunlubirponcik</t>
+  </si>
+  <si>
+    <t>regloloji</t>
+  </si>
+  <si>
+    <t>saykodelipaylasimlarr</t>
+  </si>
+  <si>
+    <t>oldvayn</t>
+  </si>
+  <si>
+    <t>futbolsokagiii</t>
+  </si>
+  <si>
+    <t>krdsturkiyeburanebeklion</t>
+  </si>
+  <si>
+    <t>pelinsu_</t>
+  </si>
+  <si>
+    <t>erkekteskilati</t>
+  </si>
+  <si>
+    <t>kizlarinicsesiiii</t>
+  </si>
+  <si>
+    <t>9gaang</t>
+  </si>
+  <si>
+    <t>9geekx</t>
+  </si>
+  <si>
+    <t>bilgihane</t>
+  </si>
+  <si>
+    <t>ogrencilerinicsesi</t>
+  </si>
+  <si>
+    <t>fun4turkiye</t>
+  </si>
+  <si>
+    <t>welcometomagara</t>
+  </si>
+  <si>
+    <t>aygunestendahaguzel</t>
+  </si>
+  <si>
+    <t>cagritanerdenbilgiler</t>
+  </si>
+  <si>
+    <t>karikaturhane</t>
+  </si>
+  <si>
+    <t>tuhaafamagercekbilgiler</t>
+  </si>
+  <si>
+    <t>daha17yasinda</t>
+  </si>
+  <si>
+    <t>fatalmontage</t>
+  </si>
+  <si>
+    <t>ashmontaqe</t>
+  </si>
+  <si>
+    <t>fbiailesi</t>
+  </si>
+  <si>
+    <t>ashreyiz</t>
+  </si>
+  <si>
+    <t>cagritanervideo</t>
+  </si>
+  <si>
+    <t>eksitenpaylasimlar</t>
+  </si>
+  <si>
+    <t>amgailesi</t>
+  </si>
+  <si>
+    <t>mendeburlemur</t>
+  </si>
+  <si>
+    <t>filmegitmedenonce</t>
+  </si>
+  <si>
+    <t>cryptokemal</t>
+  </si>
+  <si>
+    <t>faytklab</t>
+  </si>
+  <si>
+    <t>komik.paylasimlar.kulubu</t>
+  </si>
+  <si>
+    <t>butunsirribozdun</t>
+  </si>
+  <si>
+    <t>pintipanda</t>
+  </si>
+  <si>
+    <t>gidadedektifi</t>
+  </si>
+  <si>
+    <t>cezmikalorifer</t>
+  </si>
+  <si>
+    <t>incicaps</t>
+  </si>
+  <si>
+    <t>aogofficial</t>
+  </si>
+  <si>
+    <t>gzt</t>
+  </si>
+  <si>
+    <t>besiktas</t>
+  </si>
+  <si>
+    <t>binance</t>
+  </si>
+  <si>
+    <t>enesbatur</t>
+  </si>
+  <si>
+    <t>orkunisitmak</t>
+  </si>
+  <si>
+    <t>gorilfaruk</t>
+  </si>
+  <si>
+    <t>cmylmz</t>
+  </si>
+  <si>
+    <t>jahrein</t>
+  </si>
+  <si>
+    <t>trabzonspor</t>
+  </si>
+  <si>
+    <t>galatasaray</t>
+  </si>
+  <si>
+    <t>7le4ves</t>
+  </si>
+  <si>
+    <t>turklerin50tonuofficial</t>
+  </si>
+  <si>
+    <t>deliyizcunku</t>
+  </si>
+  <si>
+    <t>melihgokcekresmi</t>
+  </si>
+  <si>
+    <t>berkingham</t>
+  </si>
+  <si>
+    <t>bi2cumle</t>
+  </si>
+  <si>
+    <t>mubiturkiye</t>
+  </si>
+  <si>
+    <t>geniuskender</t>
+  </si>
+  <si>
+    <t>alperrende</t>
+  </si>
+  <si>
+    <t>rifki.baba</t>
+  </si>
+  <si>
+    <t>oykuberkan</t>
+  </si>
+  <si>
+    <t>tasarimcidayi</t>
+  </si>
+  <si>
+    <t>hakki_alkan</t>
+  </si>
+  <si>
+    <t>shiftdeletenet</t>
+  </si>
+  <si>
+    <t>kozmikagac</t>
+  </si>
+  <si>
+    <t>danlabilic</t>
+  </si>
+  <si>
+    <t>tahaozer</t>
+  </si>
+  <si>
+    <t>supervideolar</t>
+  </si>
+  <si>
+    <t>sahangokbakar</t>
+  </si>
+  <si>
+    <t>tam1lavuk</t>
+  </si>
+  <si>
+    <t>ogrenciteskilati</t>
+  </si>
+  <si>
+    <t>sozmuhendisi</t>
+  </si>
+  <si>
+    <t>agir_mizahi</t>
+  </si>
+  <si>
+    <t>saykoturkeys</t>
+  </si>
+  <si>
+    <t>girisimcikafasi</t>
+  </si>
+  <si>
+    <t>1soru.1cevap</t>
+  </si>
+  <si>
+    <t>mizah</t>
   </si>
 </sst>
 </file>
@@ -396,15 +624,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D078D2F8-6659-F149-B08A-ABEA7C55945D}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -414,12 +642,397 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>